<commit_message>
Add option to include fine scale spatial coverage.
</commit_message>
<xml_diff>
--- a/inst/templates/datasetname_spatial_bounds.xlsx
+++ b/inst/templates/datasetname_spatial_bounds.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colin\Documents\EDI\data_sets\blank\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colin\Documents\EDI\r\EMLtools\inst\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -393,7 +393,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -403,6 +403,7 @@
     <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>